<commit_message>
updated README and test_result, will do Apr_figure later
</commit_message>
<xml_diff>
--- a/files/apriori_result.xlsx
+++ b/files/apriori_result.xlsx
@@ -393,7 +393,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>905</v>
+        <v>967</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -409,7 +409,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>855</v>
+        <v>900</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -425,7 +425,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1336</v>
+        <v>1437</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -441,7 +441,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>791</v>
+        <v>847</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1013</v>
+        <v>1094</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>823</v>
+        <v>878</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1046</v>
+        <v>1106</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
@@ -501,11 +501,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>20972</t>
+          <t>21034</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>743</v>
+        <v>1072</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -517,11 +517,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>21034</t>
+          <t>21080</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1023</v>
+        <v>1078</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -533,11 +533,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21080</t>
+          <t>21175</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1007</v>
+        <v>858</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -549,11 +549,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21175</t>
+          <t>21181</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>803</v>
+        <v>980</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -565,11 +565,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21181</t>
+          <t>21212</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>913</v>
+        <v>1638</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -581,11 +581,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21212</t>
+          <t>21231</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1526</v>
+        <v>997</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -597,11 +597,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21231</t>
+          <t>21232</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>947</v>
+        <v>1655</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -613,11 +613,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21232</t>
+          <t>21621</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1550</v>
+        <v>823</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -629,11 +629,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>21621</t>
+          <t>21733</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>775</v>
+        <v>1033</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
@@ -645,11 +645,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21733</t>
+          <t>21754</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>949</v>
+        <v>1302</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -661,11 +661,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21754</t>
+          <t>21755</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1211</v>
+        <v>1082</v>
       </c>
       <c r="D19" t="n">
         <v>1</v>
@@ -677,11 +677,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>21755</t>
+          <t>21790</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1001</v>
+        <v>959</v>
       </c>
       <c r="D20" t="n">
         <v>1</v>
@@ -693,11 +693,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21790</t>
+          <t>21843</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>907</v>
+        <v>1007</v>
       </c>
       <c r="D21" t="n">
         <v>1</v>
@@ -709,11 +709,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21843</t>
+          <t>21931</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>953</v>
+        <v>1148</v>
       </c>
       <c r="D22" t="n">
         <v>1</v>
@@ -725,11 +725,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21931</t>
+          <t>21977</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1066</v>
+        <v>1046</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -741,11 +741,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>21977</t>
+          <t>22086</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>975</v>
+        <v>941</v>
       </c>
       <c r="D24" t="n">
         <v>1</v>
@@ -757,11 +757,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>22086</t>
+          <t>22090</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>882</v>
+        <v>827</v>
       </c>
       <c r="D25" t="n">
         <v>1</v>
@@ -773,11 +773,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>22090</t>
+          <t>22111</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>770</v>
+        <v>958</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
@@ -789,11 +789,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>22111</t>
+          <t>22112</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>891</v>
+        <v>899</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
@@ -805,11 +805,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>22112</t>
+          <t>22114</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>843</v>
+        <v>964</v>
       </c>
       <c r="D28" t="n">
         <v>1</v>
@@ -821,11 +821,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>22114</t>
+          <t>22138</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>889</v>
+        <v>1010</v>
       </c>
       <c r="D29" t="n">
         <v>1</v>
@@ -837,11 +837,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>22138</t>
+          <t>22139</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>961</v>
+        <v>1056</v>
       </c>
       <c r="D30" t="n">
         <v>1</v>
@@ -853,11 +853,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>22139</t>
+          <t>22149</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1000</v>
+        <v>843</v>
       </c>
       <c r="D31" t="n">
         <v>1</v>
@@ -869,11 +869,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>22149</t>
+          <t>22178</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>784</v>
+        <v>801</v>
       </c>
       <c r="D32" t="n">
         <v>1</v>
@@ -885,11 +885,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>22178</t>
+          <t>22197</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>757</v>
+        <v>969</v>
       </c>
       <c r="D33" t="n">
         <v>1</v>
@@ -901,11 +901,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>22197</t>
+          <t>22355</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>903</v>
+        <v>818</v>
       </c>
       <c r="D34" t="n">
         <v>1</v>
@@ -917,11 +917,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>22355</t>
+          <t>22382</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>767</v>
+        <v>942</v>
       </c>
       <c r="D35" t="n">
         <v>1</v>
@@ -933,11 +933,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>22382</t>
+          <t>22383</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>876</v>
+        <v>1072</v>
       </c>
       <c r="D36" t="n">
         <v>1</v>
@@ -949,11 +949,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>22383</t>
+          <t>22384</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1002</v>
+        <v>982</v>
       </c>
       <c r="D37" t="n">
         <v>1</v>
@@ -965,11 +965,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>22384</t>
+          <t>22386</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>908</v>
+        <v>1001</v>
       </c>
       <c r="D38" t="n">
         <v>1</v>
@@ -981,11 +981,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>22386</t>
+          <t>22411</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>919</v>
+        <v>1023</v>
       </c>
       <c r="D39" t="n">
         <v>1</v>
@@ -997,11 +997,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>22411</t>
+          <t>22423</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>958</v>
+        <v>1988</v>
       </c>
       <c r="D40" t="n">
         <v>1</v>
@@ -1013,11 +1013,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>22423</t>
+          <t>22457</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1887</v>
+        <v>833</v>
       </c>
       <c r="D41" t="n">
         <v>1</v>
@@ -1029,11 +1029,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>22457</t>
+          <t>22469</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>790</v>
+        <v>1024</v>
       </c>
       <c r="D42" t="n">
         <v>1</v>
@@ -1045,11 +1045,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>22469</t>
+          <t>22470</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>955</v>
+        <v>1093</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
@@ -1061,11 +1061,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>22470</t>
+          <t>47566</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1015</v>
+        <v>969</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
@@ -1077,11 +1077,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>47566</t>
+          <t>48138</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>908</v>
+        <v>1043</v>
       </c>
       <c r="D45" t="n">
         <v>1</v>
@@ -1093,11 +1093,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>48138</t>
+          <t>82482</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>991</v>
+        <v>932</v>
       </c>
       <c r="D46" t="n">
         <v>1</v>
@@ -1109,11 +1109,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>82482</t>
+          <t>82494L</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>846</v>
+        <v>1104</v>
       </c>
       <c r="D47" t="n">
         <v>1</v>
@@ -1125,11 +1125,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>82494L</t>
+          <t>84836</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1034</v>
+        <v>872</v>
       </c>
       <c r="D48" t="n">
         <v>1</v>
@@ -1141,11 +1141,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>84836</t>
+          <t>84879</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>809</v>
+        <v>1345</v>
       </c>
       <c r="D49" t="n">
         <v>1</v>
@@ -1157,11 +1157,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>84879</t>
+          <t>84946</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1246</v>
+        <v>903</v>
       </c>
       <c r="D50" t="n">
         <v>1</v>
@@ -1173,11 +1173,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>84946</t>
+          <t>84970S</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>824</v>
+        <v>866</v>
       </c>
       <c r="D51" t="n">
         <v>1</v>
@@ -1189,11 +1189,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>84970S</t>
+          <t>84991</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>811</v>
+        <v>1221</v>
       </c>
       <c r="D52" t="n">
         <v>1</v>
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>84991</t>
+          <t>84992</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1128</v>
+        <v>806</v>
       </c>
       <c r="D53" t="n">
         <v>1</v>
@@ -1225,7 +1225,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1743</v>
+        <v>1884</v>
       </c>
       <c r="D54" t="n">
         <v>1</v>
@@ -1241,7 +1241,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>879</v>
+        <v>949</v>
       </c>
       <c r="D55" t="n">
         <v>1</v>
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>951</v>
+        <v>1015</v>
       </c>
       <c r="D56" t="n">
         <v>1</v>
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>3079</v>
+        <v>3262</v>
       </c>
       <c r="D57" t="n">
         <v>1</v>

</xml_diff>